<commit_message>
Scenarij za registraciju agencije
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/RegistracijaAgencije_Scenarij.xlsx
+++ b/UseCaseIScenarij/RegistracijaAgencije_Scenarij.xlsx
@@ -29,21 +29,6 @@
     <t>Scenarij 2</t>
   </si>
   <si>
-    <t>Naziv: Registracija agencije na stranicu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opis: Ako agencija odluči da želi kreirati i reklamirati putovanja preko naše stranice mora da kreira račun. Vrši se unos podataka, te se provjerava njihova ispravnost. Ako je sve ispravno završeno je kreiranje računa. Kada se prijavi na račun pojavljuje se forma preko koje može da kreira putovanja tj.odabir destinacije,datum i vrijeme,hotel i let. Ako se odluči da kreira vrši se provjera kapaciteta i plaća određeni procenat. Agencija ne mora kreirati odma putovanja, može i da pogleda svoja prethodno kreirana.  </t>
-  </si>
-  <si>
-    <t>Glavni tok: Agencija kreira račun i kreira putovanje</t>
-  </si>
-  <si>
-    <t>Preduvjeti: Agencija mora imati račun na stranici</t>
-  </si>
-  <si>
-    <t>Posljedice: Ako odluči da otkaže putovanje procenti koje je već uplatila se ne vraćaju, jer su hotel i avio kompanija već izgubile klijente zbog rezervacije.</t>
-  </si>
-  <si>
     <t>Agencija</t>
   </si>
   <si>
@@ -62,9 +47,6 @@
     <t>1. Popunjavanje podataka</t>
   </si>
   <si>
-    <t>2. Porvjera validnosti</t>
-  </si>
-  <si>
     <t>Za korak 2</t>
   </si>
   <si>
@@ -114,6 +96,134 @@
   </si>
   <si>
     <t>11. Postavljanje na stranicu</t>
+  </si>
+  <si>
+    <t>2. Provjera validnosti</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Naziv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Registracija agencije na stranicu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Opis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Ako agencija odluči da želi kreirati i reklamirati putovanja preko naše stranice mora da kreira račun. Vrši se unos podataka, te se provjerava njihova ispravnost. Ako je sve ispravno završeno je kreiranje računa. Kada se prijavi na račun pojavljuje se forma preko koje može da kreira putovanja tj.odabir destinacije,datum i vrijeme,hotel i let. Ako se odluči da kreira vrši se provjera kapaciteta i plaća određeni procenat. Agencija ne mora kreirati odma putovanja, može i da pogleda svoja prethodno kreirana.  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Glavni tok</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Agencija kreira račun i kreira putovanje</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Preduvjeti</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Agencija mora imati račun na stranici</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Posljedice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Ako odluči da otkaže putovanje procenti koje je već uplatila se ne vraćaju, jer su hotel i avio kompanija već izgubile klijente zbog rezervacije.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -159,9 +269,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,170 +590,173 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="2" max="2" width="8.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.21875" customWidth="1"/>
+    <col min="4" max="4" width="41.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>2</v>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>3</v>
+      <c r="D5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>5</v>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>